<commit_message>
sauvegarder tâche du jour
</commit_message>
<xml_diff>
--- a/Journée d'activité/Thomas.xlsx
+++ b/Journée d'activité/Thomas.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3096DB42-2C6F-4D90-AB81-66B80FAB9759}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68A0A3E-26FF-4B0C-B363-B4C264ED470D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>DATE</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>Choix des themes/Choix des tables de BDD/Nom des Pages HTML/Shéma de l'acheminement des pages/Création de la page "end.html"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Continuer la page ""end.html"/Essaye d'intégrer le PHP à la page </t>
   </si>
 </sst>
 </file>
@@ -212,7 +215,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -245,7 +248,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -531,7 +534,7 @@
   <dimension ref="B1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T22" sqref="T22"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,7 +557,7 @@
       <c r="H2" s="12"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="13">
+      <c r="B3" s="2">
         <v>43756</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -576,7 +579,7 @@
       <c r="H4" s="9"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="13">
+      <c r="B5" s="2">
         <v>43777</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -598,7 +601,7 @@
       <c r="H6" s="9"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="13">
+      <c r="B7" s="2">
         <v>43784</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -620,8 +623,12 @@
       <c r="H8" s="9"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="4"/>
+      <c r="B9" s="2">
+        <v>43791</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
@@ -638,7 +645,7 @@
       <c r="H10" s="9"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="4"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -656,7 +663,7 @@
       <c r="H12" s="9"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="4"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
@@ -674,7 +681,7 @@
       <c r="H14" s="9"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
+      <c r="B15" s="13"/>
       <c r="C15" s="4"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -692,7 +699,7 @@
       <c r="H16" s="9"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
+      <c r="B17" s="13"/>
       <c r="C17" s="4"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -710,7 +717,7 @@
       <c r="H18" s="9"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
+      <c r="B19" s="13"/>
       <c r="C19" s="4"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -728,7 +735,7 @@
       <c r="H20" s="9"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="4"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
@@ -746,7 +753,7 @@
       <c r="H22" s="9"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
+      <c r="B23" s="13"/>
       <c r="C23" s="4"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
@@ -764,7 +771,7 @@
       <c r="H24" s="9"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
+      <c r="B25" s="13"/>
       <c r="C25" s="4"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
@@ -782,7 +789,7 @@
       <c r="H26" s="9"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
+      <c r="B27" s="13"/>
       <c r="C27" s="4"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
@@ -800,7 +807,7 @@
       <c r="H28" s="9"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="2"/>
+      <c r="B29" s="13"/>
       <c r="C29" s="4"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
@@ -818,7 +825,7 @@
       <c r="H30" s="9"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
+      <c r="B31" s="13"/>
       <c r="C31" s="4"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
@@ -837,6 +844,30 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:H28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:H30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:H32"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:H22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:H24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:H26"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:H16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:H18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:H20"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:H10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:H12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:H14"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:H8"/>
     <mergeCell ref="C2:H2"/>
@@ -844,30 +875,6 @@
     <mergeCell ref="C3:H4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:H6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:H10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:H12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:H14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:H16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:H18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:H20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:H22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:H24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:H26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:H28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:H30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:H32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Mise a jour de "journée d'activité"
</commit_message>
<xml_diff>
--- a/Journée d'activité/Thomas.xlsx
+++ b/Journée d'activité/Thomas.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2661FAD-3F26-4A6A-8C3A-4E59C4E45C72}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A9B6DA-A5F0-4C98-A071-2BE0BBE8BEDC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>DATE</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>Faire des recherches pour envoyer un socket au serveur gagner.</t>
+  </si>
+  <si>
+    <t>Récupérer le score de l'utilisateur et l'afficher sur la page de classement.</t>
   </si>
 </sst>
 </file>
@@ -580,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:H18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,8 +777,12 @@
       <c r="H18" s="9"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="15"/>
-      <c r="C19" s="4"/>
+      <c r="B19" s="2">
+        <v>43805</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>

</xml_diff>